<commit_message>
Create Usability Study; Update sprint backlog
</commit_message>
<xml_diff>
--- a/Deliverables/PALSS_Deliverable_4/PALSS_Deliverable_4_SprintBacklog.xlsx
+++ b/Deliverables/PALSS_Deliverable_4/PALSS_Deliverable_4_SprintBacklog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD531DDB-650D-4AA0-B251-E743B70B15C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23845FFA-A04B-49C3-BEA8-81341559A774}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5172" yWindow="1632" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="876" yWindow="2064" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>001</t>
   </si>
@@ -128,6 +128,36 @@
   </si>
   <si>
     <t>Technical work</t>
+  </si>
+  <si>
+    <t>Aiden</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Durgin</t>
+  </si>
+  <si>
+    <t>Matt A</t>
+  </si>
+  <si>
+    <t>Matt P</t>
+  </si>
+  <si>
+    <t>Linked FireAuth</t>
+  </si>
+  <si>
+    <t>Domain coding</t>
+  </si>
+  <si>
+    <t>Charge subtypes</t>
+  </si>
+  <si>
+    <t>UI/Domain code</t>
+  </si>
+  <si>
+    <t>Configuration</t>
   </si>
 </sst>
 </file>
@@ -481,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -543,6 +573,12 @@
       <c r="F2">
         <v>20</v>
       </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -583,6 +619,12 @@
       <c r="F4">
         <v>15</v>
       </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -603,6 +645,12 @@
       <c r="F5">
         <v>5</v>
       </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -663,6 +711,12 @@
       <c r="F8">
         <v>5</v>
       </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -702,6 +756,12 @@
       </c>
       <c r="F10">
         <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">

</xml_diff>